<commit_message>
galacticPubs::publish() [2022-07-15 23:24:14]  All projects rebuilt with DefaultLocale
</commit_message>
<xml_diff>
--- a/meta/teaching-materials.xlsx
+++ b/meta/teaching-materials.xlsx
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="111">
   <si>
     <t>Summary of Teaching Resources for Classroom &amp; Remote</t>
   </si>
@@ -520,6 +520,42 @@
   <si>
     <t>1b5pBKdYlMukFkCQjwposyRHdL3QMrq3-tgskbRXGkgo</t>
   </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>P1_Classroom-Set_Image Cards</t>
+  </si>
+  <si>
+    <t>WhatIsBeauty_P1_G5-8_wksht (TEACHER)</t>
+  </si>
+  <si>
+    <t>WhatIsBeauty_P3_G5-8_wksht</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/13N7umQ-WH3RmTcFLd5DmbnnpwrJzMb2bDeAw7ZByl7o/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/15hLhB4OU-DV1vEsJjOrXBcb5smhceC3ssGyOHKPO4B0/edit?usp=drivesdk</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/13N7umQ-WH3RmTcFLd5DmbnnpwrJzMb2bDeAw7ZByl7o/</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/15hLhB4OU-DV1vEsJjOrXBcb5smhceC3ssGyOHKPO4B0/</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/13N7umQ-WH3RmTcFLd5DmbnnpwrJzMb2bDeAw7ZByl7o/export?format=pdf</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/document/d/15hLhB4OU-DV1vEsJjOrXBcb5smhceC3ssGyOHKPO4B0/export?format=pdf</t>
+  </si>
+  <si>
+    <t>13N7umQ-WH3RmTcFLd5DmbnnpwrJzMb2bDeAw7ZByl7o</t>
+  </si>
+  <si>
+    <t>15hLhB4OU-DV1vEsJjOrXBcb5smhceC3ssGyOHKPO4B0</t>
+  </si>
 </sst>
 </file>
 
@@ -823,7 +859,7 @@
       <alignment wrapText="true"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="307">
+  <cellXfs count="475">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -957,6 +993,510 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
+      <alignment wrapText="true"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2">
       <alignment wrapText="true"/>
     </xf>
@@ -4775,44 +5315,44 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="259" t="s">
+      <c r="A3" s="419" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="261" t="s">
+      <c r="B3" s="421" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="263" t="s">
+      <c r="C3" s="423" t="s">
         <v>64</v>
       </c>
-      <c r="D3" s="265" t="s">
+      <c r="D3" s="425" t="s">
         <v>65</v>
       </c>
-      <c r="E3" s="267" t="s">
+      <c r="E3" s="427" t="s">
         <v>67</v>
       </c>
       <c r="F3" s="14"/>
-      <c r="G3" t="s" s="269">
+      <c r="G3" t="s" s="429">
         <v>69</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="260" t="s">
+      <c r="A4" s="420" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="262" t="s">
+      <c r="B4" s="422" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="264" t="s">
+      <c r="C4" s="424" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="266" t="s">
+      <c r="D4" s="426" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="268" t="s">
+      <c r="E4" s="428" t="s">
         <v>68</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" t="s" s="270">
+      <c r="G4" t="s" s="430">
         <v>70</v>
       </c>
     </row>
@@ -5966,54 +6506,54 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="271" t="s">
+      <c r="C3" s="431" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="273" t="s">
+      <c r="D3" s="433" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="275" t="s">
+      <c r="E3" s="435" t="s">
         <v>74</v>
       </c>
-      <c r="F3" s="277" t="s">
+      <c r="F3" s="437" t="s">
         <v>75</v>
       </c>
       <c r="G3" s="14"/>
-      <c r="H3" s="279" t="s">
+      <c r="H3" s="439" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="281" t="s">
+      <c r="I3" s="441" t="s">
         <v>79</v>
       </c>
       <c r="J3"/>
-      <c r="K3" t="s" s="283">
+      <c r="K3" t="s" s="443">
         <v>81</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="272" t="s">
+      <c r="C4" s="432" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="274" t="s">
+      <c r="D4" s="434" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="276" t="s">
+      <c r="E4" s="436" t="s">
         <v>73</v>
       </c>
-      <c r="F4" s="278" t="s">
+      <c r="F4" s="438" t="s">
         <v>76</v>
       </c>
       <c r="G4" s="14"/>
-      <c r="H4" s="280" t="s">
+      <c r="H4" s="440" t="s">
         <v>78</v>
       </c>
-      <c r="I4" s="282" t="s">
+      <c r="I4" s="442" t="s">
         <v>80</v>
       </c>
       <c r="J4"/>
-      <c r="K4" t="s" s="284">
+      <c r="K4" t="s" s="444">
         <v>82</v>
       </c>
     </row>
@@ -7578,29 +8118,31 @@
     <row r="3">
       <c r="A3" s="23"/>
       <c r="B3"/>
-      <c r="C3" s="285" t="s">
+      <c r="C3" s="445" t="s">
         <v>63</v>
       </c>
-      <c r="D3" s="288" t="s">
+      <c r="D3" s="449" t="s">
         <v>71</v>
       </c>
-      <c r="E3" s="14"/>
+      <c r="E3" s="453" t="s">
+        <v>84</v>
+      </c>
       <c r="F3" s="14"/>
-      <c r="G3" s="292" t="s">
-        <v>83</v>
+      <c r="G3" s="455" t="s">
+        <v>101</v>
       </c>
-      <c r="H3" s="295" t="s">
-        <v>87</v>
+      <c r="H3" s="459" t="s">
+        <v>103</v>
       </c>
       <c r="I3" s="14"/>
-      <c r="J3" s="298" t="s">
-        <v>90</v>
+      <c r="J3" s="463" t="s">
+        <v>105</v>
       </c>
-      <c r="K3" s="301" t="s">
-        <v>93</v>
+      <c r="K3" s="467" t="s">
+        <v>107</v>
       </c>
-      <c r="L3" t="s" s="304">
-        <v>96</v>
+      <c r="L3" t="s" s="471">
+        <v>109</v>
       </c>
       <c r="U3" s="9"/>
       <c r="V3" s="9"/>
@@ -7613,30 +8155,30 @@
     <row r="4">
       <c r="A4" s="23"/>
       <c r="B4"/>
-      <c r="C4" s="286" t="s">
+      <c r="C4" s="446" t="s">
         <v>63</v>
       </c>
-      <c r="D4" s="289" t="s">
+      <c r="D4" s="450" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="291" t="s">
+      <c r="E4" s="454" t="s">
         <v>84</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="293" t="s">
+      <c r="G4" s="456" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="296" t="s">
+      <c r="H4" s="460" t="s">
         <v>88</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="299" t="s">
+      <c r="J4" s="464" t="s">
         <v>91</v>
       </c>
-      <c r="K4" s="302" t="s">
+      <c r="K4" s="468" t="s">
         <v>94</v>
       </c>
-      <c r="L4" t="s" s="305">
+      <c r="L4" t="s" s="472">
         <v>97</v>
       </c>
       <c r="U4" s="9"/>
@@ -7650,29 +8192,29 @@
     <row r="5">
       <c r="A5" s="23"/>
       <c r="B5"/>
-      <c r="C5" s="287" t="s">
+      <c r="C5" s="447" t="s">
         <v>63</v>
       </c>
-      <c r="D5" s="290" t="s">
-        <v>83</v>
+      <c r="D5" s="451" t="s">
+        <v>99</v>
       </c>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
-      <c r="G5" s="294" t="s">
-        <v>85</v>
+      <c r="G5" s="457" t="s">
+        <v>102</v>
       </c>
-      <c r="H5" s="297" t="s">
-        <v>89</v>
+      <c r="H5" s="461" t="s">
+        <v>104</v>
       </c>
       <c r="I5" s="14"/>
-      <c r="J5" s="300" t="s">
-        <v>92</v>
+      <c r="J5" s="465" t="s">
+        <v>106</v>
       </c>
-      <c r="K5" s="303" t="s">
-        <v>95</v>
+      <c r="K5" s="469" t="s">
+        <v>108</v>
       </c>
-      <c r="L5" t="s" s="306">
-        <v>98</v>
+      <c r="L5" t="s" s="473">
+        <v>110</v>
       </c>
       <c r="U5" s="9"/>
       <c r="V5" s="9"/>
@@ -7684,15 +8226,31 @@
     </row>
     <row r="6">
       <c r="A6" s="23"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
+      <c r="B6"/>
+      <c r="C6" s="448" t="s">
+        <v>63</v>
+      </c>
+      <c r="D6" s="452" t="s">
+        <v>100</v>
+      </c>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
+      <c r="G6" s="458" t="s">
+        <v>100</v>
+      </c>
+      <c r="H6" s="462" t="s">
+        <v>89</v>
+      </c>
       <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
+      <c r="J6" s="466" t="s">
+        <v>92</v>
+      </c>
+      <c r="K6" s="470" t="s">
+        <v>95</v>
+      </c>
+      <c r="L6" t="s" s="474">
+        <v>98</v>
+      </c>
       <c r="U6" s="9"/>
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>

</xml_diff>